<commit_message>
Entrenameinto de modelos priemra fase
</commit_message>
<xml_diff>
--- a/data/clean/MJ/MJ-JUNIO-2024_features.xlsx
+++ b/data/clean/MJ/MJ-JUNIO-2024_features.xlsx
@@ -487,7 +487,7 @@
         <v>-0.3017758983757586</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G2" t="n">
         <v>300000</v>
@@ -510,7 +510,7 @@
         <v>0.2859410534928541</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G3" t="n">
         <v>70000</v>
@@ -533,7 +533,7 @@
         <v>-0.3107769688097825</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G4" t="n">
         <v>140000</v>
@@ -556,7 +556,7 @@
         <v>-0.3107769688097825</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G5" t="n">
         <v>60000</v>
@@ -579,7 +579,7 @@
         <v>-0.3107769688097825</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G6" t="n">
         <v>50000</v>
@@ -602,7 +602,7 @@
         <v>-0.3107769688097825</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G7" t="n">
         <v>25000</v>
@@ -625,7 +625,7 @@
         <v>-0.3271906854835905</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G8" t="n">
         <v>85000</v>
@@ -648,7 +648,7 @@
         <v>-0.3420159779631591</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G9" t="n">
         <v>95000</v>
@@ -671,7 +671,7 @@
         <v>-0.1651714176711622</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G10" t="n">
         <v>55000</v>
@@ -694,7 +694,7 @@
         <v>-0.5204489624493956</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G11" t="n">
         <v>38000</v>
@@ -717,7 +717,7 @@
         <v>-0.5204489624493956</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G12" t="n">
         <v>65000</v>
@@ -740,7 +740,7 @@
         <v>-0.5516879716027723</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G13" t="n">
         <v>60000</v>
@@ -763,7 +763,7 @@
         <v>-0.6326976055089865</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G14" t="n">
         <v>85000</v>
@@ -786,7 +786,7 @@
         <v>-0.6326976055089865</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G15" t="n">
         <v>50000</v>
@@ -809,7 +809,7 @@
         <v>-0.7290620066261825</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G16" t="n">
         <v>95000</v>
@@ -832,7 +832,7 @@
         <v>-0.4876215291017794</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G17" t="n">
         <v>50000</v>
@@ -855,7 +855,7 @@
         <v>-0.3107769688097825</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G18" t="n">
         <v>170000</v>
@@ -878,7 +878,7 @@
         <v>3.041327555766962</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G19" t="n">
         <v>75000</v>
@@ -901,7 +901,7 @@
         <v>-0.5516879716027723</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G20" t="n">
         <v>25000</v>
@@ -924,7 +924,7 @@
         <v>3.041857030498375</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G21" t="n">
         <v>35000</v>
@@ -947,7 +947,7 @@
         <v>1.848950460624516</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G22" t="n">
         <v>35000</v>
@@ -970,7 +970,7 @@
         <v>3.041327555766962</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G23" t="n">
         <v>35000</v>
@@ -993,7 +993,7 @@
         <v>3.090568705788386</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G24" t="n">
         <v>22000</v>
@@ -1016,7 +1016,7 @@
         <v>-0.06880701655396622</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G25" t="n">
         <v>31500</v>
@@ -1039,7 +1039,7 @@
         <v>-0.5675722135451673</v>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G26" t="n">
         <v>25000</v>
@@ -1062,7 +1062,7 @@
         <v>-0.5998701721613703</v>
       </c>
       <c r="F27" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G27" t="n">
         <v>30000</v>
@@ -1085,7 +1085,7 @@
         <v>-0.04498065364037385</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G28" t="n">
         <v>200000</v>
@@ -1108,7 +1108,7 @@
         <v>-0.1175186918439774</v>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G29" t="n">
         <v>21000</v>
@@ -1131,7 +1131,7 @@
         <v>-0.4717372871593844</v>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G30" t="n">
         <v>35000</v>
@@ -1154,7 +1154,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G31" t="n">
         <v>20000</v>
@@ -1177,7 +1177,7 @@
         <v>2.976202163803143</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G32" t="n">
         <v>22000</v>
@@ -1200,7 +1200,7 @@
         <v>2.391662060323009</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G33" t="n">
         <v>36000</v>
@@ -1223,7 +1223,7 @@
         <v>2.391662060323009</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G34" t="n">
         <v>22000</v>
@@ -1246,7 +1246,7 @@
         <v>-0.4066118951955652</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G35" t="n">
         <v>70000</v>
@@ -1269,7 +1269,7 @@
         <v>-0.5675722135451673</v>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G36" t="n">
         <v>32000</v>
@@ -1292,7 +1292,7 @@
         <v>-0.5998701721613703</v>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G37" t="n">
         <v>110000</v>
@@ -1315,7 +1315,7 @@
         <v>-0.6649955641251896</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G38" t="n">
         <v>35000</v>
@@ -1338,7 +1338,7 @@
         <v>2.267764973172329</v>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G39" t="n">
         <v>26250</v>
@@ -1361,7 +1361,7 @@
         <v>0.2059903690494662</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G40" t="n">
         <v>50000</v>
@@ -1384,7 +1384,7 @@
         <v>2.267764973172329</v>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G41" t="n">
         <v>36000</v>
@@ -1407,7 +1407,7 @@
         <v>3.041327555766962</v>
       </c>
       <c r="F42" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G42" t="n">
         <v>24066.26</v>
@@ -1430,7 +1430,7 @@
         <v>-0.1974693762873652</v>
       </c>
       <c r="F43" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G43" t="n">
         <v>49000</v>
@@ -1453,7 +1453,7 @@
         <v>-0.1974693762873652</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G44" t="n">
         <v>40000</v>
@@ -1476,7 +1476,7 @@
         <v>-0.1974693762873652</v>
       </c>
       <c r="F45" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G45" t="n">
         <v>35000</v>
@@ -1499,7 +1499,7 @@
         <v>-0.3271906854835905</v>
       </c>
       <c r="F46" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G46" t="n">
         <v>37333.33</v>
@@ -1522,7 +1522,7 @@
         <v>-0.3584296946369672</v>
       </c>
       <c r="F47" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G47" t="n">
         <v>35000</v>
@@ -1545,7 +1545,7 @@
         <v>-0.4553235704855764</v>
       </c>
       <c r="F48" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G48" t="n">
         <v>26500</v>
@@ -1568,7 +1568,7 @@
         <v>-0.5204489624493956</v>
       </c>
       <c r="F49" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G49" t="n">
         <v>38000</v>
@@ -1591,7 +1591,7 @@
         <v>-0.5204489624493956</v>
       </c>
       <c r="F50" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G50" t="n">
         <v>35000</v>
@@ -1614,7 +1614,7 @@
         <v>-0.5675722135451673</v>
       </c>
       <c r="F51" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G51" t="n">
         <v>30000</v>
@@ -1637,7 +1637,7 @@
         <v>-0.3753728860421885</v>
       </c>
       <c r="F52" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G52" t="n">
         <v>38000</v>
@@ -1660,7 +1660,7 @@
         <v>-0.0529227746115713</v>
       </c>
       <c r="F53" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G53" t="n">
         <v>36000</v>
@@ -1683,7 +1683,7 @@
         <v>-0.0529227746115713</v>
       </c>
       <c r="F54" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G54" t="n">
         <v>32000</v>
@@ -1706,7 +1706,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F55" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G55" t="n">
         <v>25000</v>
@@ -1729,7 +1729,7 @@
         <v>-0.0529227746115713</v>
       </c>
       <c r="F56" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G56" t="n">
         <v>31500</v>
@@ -1752,7 +1752,7 @@
         <v>3.041327555766962</v>
       </c>
       <c r="F57" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G57" t="n">
         <v>16500</v>
@@ -1775,7 +1775,7 @@
         <v>-0.4876215291017794</v>
       </c>
       <c r="F58" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G58" t="n">
         <v>25000</v>
@@ -1798,7 +1798,7 @@
         <v>1.075387878029882</v>
       </c>
       <c r="F59" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G59" t="n">
         <v>27000</v>
@@ -1821,7 +1821,7 @@
         <v>-0.3277201602150037</v>
       </c>
       <c r="F60" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G60" t="n">
         <v>49000</v>
@@ -1844,7 +1844,7 @@
         <v>0.1085670184694439</v>
       </c>
       <c r="F61" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G61" t="n">
         <v>42000</v>
@@ -1867,7 +1867,7 @@
         <v>2.976731638534556</v>
       </c>
       <c r="F62" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G62" t="n">
         <v>21000</v>
@@ -1890,7 +1890,7 @@
         <v>-0.004211099321560156</v>
       </c>
       <c r="F63" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G63" t="n">
         <v>29521</v>
@@ -1913,7 +1913,7 @@
         <v>3.025443313824567</v>
       </c>
       <c r="F64" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G64" t="n">
         <v>35000</v>
@@ -1936,7 +1936,7 @@
         <v>-0.04498065364037385</v>
       </c>
       <c r="F65" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G65" t="n">
         <v>31500</v>
@@ -1959,7 +1959,7 @@
         <v>3.041327555766962</v>
       </c>
       <c r="F66" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G66" t="n">
         <v>31500</v>
@@ -1982,7 +1982,7 @@
         <v>2.186755339266115</v>
       </c>
       <c r="F67" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G67" t="n">
         <v>120000</v>
@@ -2005,7 +2005,7 @@
         <v>-0.2382389306061789</v>
       </c>
       <c r="F68" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G68" t="n">
         <v>200000</v>
@@ -2028,7 +2028,7 @@
         <v>-0.04498065364037385</v>
       </c>
       <c r="F69" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G69" t="n">
         <v>31500</v>
@@ -2051,7 +2051,7 @@
         <v>-0.04498065364037385</v>
       </c>
       <c r="F70" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G70" t="n">
         <v>40000</v>
@@ -2074,7 +2074,7 @@
         <v>-0.6326976055089865</v>
       </c>
       <c r="F71" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G71" t="n">
         <v>20000</v>
@@ -2097,7 +2097,7 @@
         <v>-0.04498065364037385</v>
       </c>
       <c r="F72" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G72" t="n">
         <v>130000</v>
@@ -2120,7 +2120,7 @@
         <v>4.330598526758018</v>
       </c>
       <c r="F73" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G73" t="n">
         <v>22000</v>
@@ -2143,7 +2143,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F74" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G74" t="n">
         <v>35000</v>
@@ -2166,7 +2166,7 @@
         <v>2.542562358775761</v>
       </c>
       <c r="F75" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G75" t="n">
         <v>38000</v>
@@ -2189,7 +2189,7 @@
         <v>0.8016494418892764</v>
       </c>
       <c r="F76" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G76" t="n">
         <v>50000</v>
@@ -2212,7 +2212,7 @@
         <v>2.268294447903743</v>
       </c>
       <c r="F77" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G77" t="n">
         <v>100000</v>
@@ -2235,7 +2235,7 @@
         <v>2.300592406519945</v>
       </c>
       <c r="F78" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G78" t="n">
         <v>31500</v>
@@ -2258,7 +2258,7 @@
         <v>2.542562358775761</v>
       </c>
       <c r="F79" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G79" t="n">
         <v>16500</v>
@@ -2281,7 +2281,7 @@
         <v>-0.6972935227413926</v>
       </c>
       <c r="F80" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G80" t="n">
         <v>40000</v>
@@ -2304,7 +2304,7 @@
         <v>-0.0529227746115713</v>
       </c>
       <c r="F81" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G81" t="n">
         <v>30000</v>
@@ -2327,7 +2327,7 @@
         <v>-0.0529227746115713</v>
       </c>
       <c r="F82" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G82" t="n">
         <v>22000</v>
@@ -2350,7 +2350,7 @@
         <v>2.380543090963333</v>
       </c>
       <c r="F83" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G83" t="n">
         <v>21000</v>
@@ -2373,7 +2373,7 @@
         <v>2.719936393799172</v>
       </c>
       <c r="F84" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G84" t="n">
         <v>25000</v>
@@ -2396,7 +2396,7 @@
         <v>-0.1175186918439774</v>
       </c>
       <c r="F85" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G85" t="n">
         <v>25000</v>
@@ -2419,7 +2419,7 @@
         <v>-0.1339324085177854</v>
       </c>
       <c r="F86" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G86" t="n">
         <v>25000</v>
@@ -2442,7 +2442,7 @@
         <v>-0.3271906854835905</v>
       </c>
       <c r="F87" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G87" t="n">
         <v>30000</v>
@@ -2465,7 +2465,7 @@
         <v>-0.3584296946369672</v>
       </c>
       <c r="F88" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G88" t="n">
         <v>30000</v>
@@ -2488,7 +2488,7 @@
         <v>2.687638435182969</v>
       </c>
       <c r="F89" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G89" t="n">
         <v>25000</v>
@@ -2511,7 +2511,7 @@
         <v>-0.4717372871593844</v>
       </c>
       <c r="F90" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G90" t="n">
         <v>26500</v>
@@ -2534,7 +2534,7 @@
         <v>-0.5516879716027723</v>
       </c>
       <c r="F91" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G91" t="n">
         <v>25000</v>
@@ -2557,7 +2557,7 @@
         <v>-0.6649955641251896</v>
       </c>
       <c r="F92" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G92" t="n">
         <v>26000</v>
@@ -2580,7 +2580,7 @@
         <v>-0.7290620066261825</v>
       </c>
       <c r="F93" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G93" t="n">
         <v>26000</v>
@@ -2603,7 +2603,7 @@
         <v>-0.7777736819161936</v>
       </c>
       <c r="F94" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G94" t="n">
         <v>26000</v>
@@ -2626,7 +2626,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F95" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G95" t="n">
         <v>25000</v>
@@ -2649,7 +2649,7 @@
         <v>-0.1974693762873652</v>
       </c>
       <c r="F96" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G96" t="n">
         <v>80000</v>
@@ -2672,7 +2672,7 @@
         <v>-0.1974693762873652</v>
       </c>
       <c r="F97" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G97" t="n">
         <v>32000</v>
@@ -2695,7 +2695,7 @@
         <v>-0.0529227746115713</v>
       </c>
       <c r="F98" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G98" t="n">
         <v>30000</v>
@@ -2718,7 +2718,7 @@
         <v>-0.0529227746115713</v>
       </c>
       <c r="F99" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G99" t="n">
         <v>22000</v>
@@ -2741,7 +2741,7 @@
         <v>-0.0529227746115713</v>
       </c>
       <c r="F100" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G100" t="n">
         <v>30000</v>
@@ -2764,7 +2764,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F101" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G101" t="n">
         <v>18000</v>
@@ -2787,7 +2787,7 @@
         <v>2.494380158217163</v>
       </c>
       <c r="F102" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G102" t="n">
         <v>18000</v>
@@ -2810,7 +2810,7 @@
         <v>2.719936393799172</v>
       </c>
       <c r="F103" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G103" t="n">
         <v>18000</v>
@@ -2833,7 +2833,7 @@
         <v>2.542562358775761</v>
       </c>
       <c r="F104" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G104" t="n">
         <v>16500</v>
@@ -2856,7 +2856,7 @@
         <v>1.236348196379484</v>
       </c>
       <c r="F105" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G105" t="n">
         <v>10000</v>
@@ -2879,7 +2879,7 @@
         <v>2.445668482927152</v>
       </c>
       <c r="F106" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G106" t="n">
         <v>10000</v>
@@ -2902,7 +2902,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F107" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G107" t="n">
         <v>18000</v>
@@ -2925,7 +2925,7 @@
         <v>-0.3420159779631591</v>
       </c>
       <c r="F108" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G108" t="n">
         <v>38000</v>
@@ -2948,7 +2948,7 @@
         <v>-0.3753728860421885</v>
       </c>
       <c r="F109" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G109" t="n">
         <v>25000</v>
@@ -2971,7 +2971,7 @@
         <v>-0.3753728860421885</v>
       </c>
       <c r="F110" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G110" t="n">
         <v>30000</v>
@@ -2994,7 +2994,7 @@
         <v>-0.4717372871593844</v>
       </c>
       <c r="F111" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G111" t="n">
         <v>22000</v>
@@ -3017,7 +3017,7 @@
         <v>-0.4717372871593844</v>
       </c>
       <c r="F112" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G112" t="n">
         <v>22000</v>
@@ -3040,7 +3040,7 @@
         <v>-0.4717372871593844</v>
       </c>
       <c r="F113" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G113" t="n">
         <v>16500</v>
@@ -3063,7 +3063,7 @@
         <v>-0.4717372871593844</v>
       </c>
       <c r="F114" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G114" t="n">
         <v>22000</v>
@@ -3086,7 +3086,7 @@
         <v>-0.4876215291017794</v>
       </c>
       <c r="F115" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G115" t="n">
         <v>16000</v>
@@ -3109,7 +3109,7 @@
         <v>-0.4876215291017794</v>
       </c>
       <c r="F116" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G116" t="n">
         <v>20000</v>
@@ -3132,7 +3132,7 @@
         <v>-0.4876215291017794</v>
       </c>
       <c r="F117" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G117" t="n">
         <v>35000</v>
@@ -3155,7 +3155,7 @@
         <v>-0.4717372871593844</v>
       </c>
       <c r="F118" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G118" t="n">
         <v>30000</v>
@@ -3178,7 +3178,7 @@
         <v>-0.5352742549289643</v>
       </c>
       <c r="F119" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G119" t="n">
         <v>35000</v>
@@ -3201,7 +3201,7 @@
         <v>-0.5352742549289643</v>
       </c>
       <c r="F120" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G120" t="n">
         <v>25000</v>
@@ -3224,7 +3224,7 @@
         <v>-0.5516879716027723</v>
       </c>
       <c r="F121" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G121" t="n">
         <v>20000</v>
@@ -3247,7 +3247,7 @@
         <v>-0.5516879716027723</v>
       </c>
       <c r="F122" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G122" t="n">
         <v>20000</v>
@@ -3270,7 +3270,7 @@
         <v>-0.5675722135451673</v>
       </c>
       <c r="F123" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G123" t="n">
         <v>26000</v>
@@ -3293,7 +3293,7 @@
         <v>-0.3584296946369672</v>
       </c>
       <c r="F124" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G124" t="n">
         <v>50000</v>
@@ -3316,7 +3316,7 @@
         <v>-0.6649955641251896</v>
       </c>
       <c r="F125" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G125" t="n">
         <v>20000</v>
@@ -3339,7 +3339,7 @@
         <v>-0.7777736819161936</v>
       </c>
       <c r="F126" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G126" t="n">
         <v>26000</v>
@@ -3362,7 +3362,7 @@
         <v>-0.7777736819161936</v>
       </c>
       <c r="F127" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G127" t="n">
         <v>15000</v>
@@ -3385,7 +3385,7 @@
         <v>-0.1175186918439774</v>
       </c>
       <c r="F128" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G128" t="n">
         <v>30000</v>
@@ -3408,7 +3408,7 @@
         <v>1.026676202739871</v>
       </c>
       <c r="F129" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G129" t="n">
         <v>18000</v>
@@ -3431,7 +3431,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F130" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G130" t="n">
         <v>22000</v>
@@ -3454,7 +3454,7 @@
         <v>2.573801367929138</v>
       </c>
       <c r="F131" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G131" t="n">
         <v>16500</v>
@@ -3477,7 +3477,7 @@
         <v>-0.6485818474513815</v>
       </c>
       <c r="F132" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G132" t="n">
         <v>26000</v>
@@ -3500,7 +3500,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F133" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G133" t="n">
         <v>25000</v>
@@ -3523,7 +3523,7 @@
         <v>-0.1180481665753905</v>
       </c>
       <c r="F134" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G134" t="n">
         <v>30000</v>
@@ -3546,7 +3546,7 @@
         <v>2.929078912707371</v>
       </c>
       <c r="F135" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G135" t="n">
         <v>31500</v>
@@ -3569,7 +3569,7 @@
         <v>-0.0529227746115713</v>
       </c>
       <c r="F136" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G136" t="n">
         <v>31500</v>
@@ -3592,7 +3592,7 @@
         <v>-0.0529227746115713</v>
       </c>
       <c r="F137" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G137" t="n">
         <v>25000</v>
@@ -3615,7 +3615,7 @@
         <v>1.865364177298324</v>
       </c>
       <c r="F138" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G138" t="n">
         <v>22000</v>
@@ -3638,7 +3638,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F139" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G139" t="n">
         <v>25000</v>
@@ -3661,7 +3661,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F140" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G140" t="n">
         <v>22000</v>
@@ -3684,7 +3684,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F141" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G141" t="n">
         <v>25000</v>
@@ -3707,7 +3707,7 @@
         <v>-0.04498065364037385</v>
       </c>
       <c r="F142" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G142" t="n">
         <v>40000</v>
@@ -3730,7 +3730,7 @@
         <v>-0.04498065364037385</v>
       </c>
       <c r="F143" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G143" t="n">
         <v>20000</v>
@@ -3753,7 +3753,7 @@
         <v>-0.04498065364037385</v>
       </c>
       <c r="F144" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G144" t="n">
         <v>20000</v>
@@ -3776,7 +3776,7 @@
         <v>-0.1011049751701693</v>
       </c>
       <c r="F145" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G145" t="n">
         <v>15000</v>
@@ -3799,7 +3799,7 @@
         <v>-0.3271906854835905</v>
       </c>
       <c r="F146" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G146" t="n">
         <v>25000</v>
@@ -3822,7 +3822,7 @@
         <v>-0.4876215291017794</v>
       </c>
       <c r="F147" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G147" t="n">
         <v>25000</v>
@@ -3845,7 +3845,7 @@
         <v>-0.4717372871593844</v>
       </c>
       <c r="F148" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G148" t="n">
         <v>25000</v>
@@ -3868,7 +3868,7 @@
         <v>-0.5040352457755874</v>
       </c>
       <c r="F149" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G149" t="n">
         <v>25000</v>
@@ -3891,7 +3891,7 @@
         <v>-0.5204489624493956</v>
       </c>
       <c r="F150" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G150" t="n">
         <v>25000</v>
@@ -3914,7 +3914,7 @@
         <v>-0.5516879716027723</v>
       </c>
       <c r="F151" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G151" t="n">
         <v>25000</v>
@@ -3937,7 +3937,7 @@
         <v>-0.5998701721613703</v>
       </c>
       <c r="F152" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G152" t="n">
         <v>30000</v>
@@ -3960,7 +3960,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F153" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G153" t="n">
         <v>25000</v>
@@ -3983,7 +3983,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F154" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G154" t="n">
         <v>25000</v>
@@ -4006,7 +4006,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F155" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G155" t="n">
         <v>25000</v>
@@ -4029,7 +4029,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F156" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G156" t="n">
         <v>25000</v>
@@ -4052,7 +4052,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F157" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G157" t="n">
         <v>25000</v>
@@ -4075,7 +4075,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F158" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G158" t="n">
         <v>25000</v>
@@ -4098,7 +4098,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F159" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G159" t="n">
         <v>25000</v>
@@ -4121,7 +4121,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F160" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G160" t="n">
         <v>25000</v>
@@ -4144,7 +4144,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F161" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G161" t="n">
         <v>25000</v>
@@ -4167,7 +4167,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F162" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G162" t="n">
         <v>25000</v>
@@ -4190,7 +4190,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F163" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G163" t="n">
         <v>25000</v>
@@ -4213,7 +4213,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F164" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G164" t="n">
         <v>25000</v>
@@ -4236,7 +4236,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F165" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G165" t="n">
         <v>25000</v>
@@ -4259,7 +4259,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F166" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G166" t="n">
         <v>25000</v>
@@ -4282,7 +4282,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F167" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G167" t="n">
         <v>25000</v>
@@ -4305,7 +4305,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F168" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G168" t="n">
         <v>25000</v>
@@ -4328,7 +4328,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F169" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G169" t="n">
         <v>25000</v>
@@ -4351,7 +4351,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F170" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G170" t="n">
         <v>25000</v>
@@ -4374,7 +4374,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F171" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G171" t="n">
         <v>25000</v>
@@ -4397,7 +4397,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F172" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G172" t="n">
         <v>25000</v>
@@ -4420,7 +4420,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F173" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G173" t="n">
         <v>25000</v>
@@ -4443,7 +4443,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F174" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G174" t="n">
         <v>25000</v>
@@ -4466,7 +4466,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F175" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G175" t="n">
         <v>25000</v>
@@ -4489,7 +4489,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F176" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G176" t="n">
         <v>25000</v>
@@ -4512,7 +4512,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F177" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G177" t="n">
         <v>25000</v>
@@ -4535,7 +4535,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F178" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G178" t="n">
         <v>25000</v>
@@ -4558,7 +4558,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F179" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G179" t="n">
         <v>25000</v>
@@ -4581,7 +4581,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F180" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G180" t="n">
         <v>25000</v>
@@ -4604,7 +4604,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F181" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G181" t="n">
         <v>25000</v>
@@ -4627,7 +4627,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F182" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G182" t="n">
         <v>25000</v>
@@ -4650,7 +4650,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F183" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G183" t="n">
         <v>25000</v>
@@ -4673,7 +4673,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F184" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G184" t="n">
         <v>25000</v>
@@ -4696,7 +4696,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F185" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G185" t="n">
         <v>25000</v>
@@ -4719,7 +4719,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F186" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G186" t="n">
         <v>25000</v>
@@ -4742,7 +4742,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F187" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G187" t="n">
         <v>25000</v>
@@ -4765,7 +4765,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F188" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G188" t="n">
         <v>25000</v>
@@ -4788,7 +4788,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F189" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G189" t="n">
         <v>25000</v>
@@ -4811,7 +4811,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F190" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G190" t="n">
         <v>25000</v>
@@ -4834,7 +4834,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F191" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G191" t="n">
         <v>25000</v>
@@ -4857,7 +4857,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F192" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G192" t="n">
         <v>25000</v>
@@ -4880,7 +4880,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F193" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G193" t="n">
         <v>25000</v>
@@ -4903,7 +4903,7 @@
         <v>-0.6808798060675845</v>
       </c>
       <c r="F194" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G194" t="n">
         <v>25000</v>
@@ -4926,7 +4926,7 @@
         <v>-0.7290620066261825</v>
       </c>
       <c r="F195" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G195" t="n">
         <v>25000</v>
@@ -4949,7 +4949,7 @@
         <v>-0.7290620066261825</v>
       </c>
       <c r="F196" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G196" t="n">
         <v>25000</v>
@@ -4972,7 +4972,7 @@
         <v>-0.7290620066261825</v>
       </c>
       <c r="F197" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G197" t="n">
         <v>25000</v>
@@ -4995,7 +4995,7 @@
         <v>-0.7290620066261825</v>
       </c>
       <c r="F198" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G198" t="n">
         <v>25000</v>
@@ -5018,7 +5018,7 @@
         <v>-0.04445117890896069</v>
       </c>
       <c r="F199" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G199" t="n">
         <v>200000</v>
@@ -5041,7 +5041,7 @@
         <v>-0.0529227746115713</v>
       </c>
       <c r="F200" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G200" t="n">
         <v>31500</v>
@@ -5064,7 +5064,7 @@
         <v>-0.0529227746115713</v>
       </c>
       <c r="F201" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G201" t="n">
         <v>40000</v>
@@ -5087,7 +5087,7 @@
         <v>-0.1974693762873652</v>
       </c>
       <c r="F202" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G202" t="n">
         <v>25000</v>
@@ -5110,7 +5110,7 @@
         <v>-0.7290620066261825</v>
       </c>
       <c r="F203" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G203" t="n">
         <v>25000</v>
@@ -5133,7 +5133,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F204" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G204" t="n">
         <v>25000</v>
@@ -5156,7 +5156,7 @@
         <v>2.960317921860748</v>
       </c>
       <c r="F205" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G205" t="n">
         <v>30000</v>
@@ -5179,7 +5179,7 @@
         <v>2.251880731229934</v>
       </c>
       <c r="F206" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G206" t="n">
         <v>45000</v>
@@ -5202,7 +5202,7 @@
         <v>2.235467014556126</v>
       </c>
       <c r="F207" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G207" t="n">
         <v>31500</v>
@@ -5225,7 +5225,7 @@
         <v>-0.4066118951955652</v>
       </c>
       <c r="F208" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G208" t="n">
         <v>30000</v>
@@ -5248,7 +5248,7 @@
         <v>-0.5998701721613703</v>
       </c>
       <c r="F209" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G209" t="n">
         <v>25000</v>
@@ -5271,7 +5271,7 @@
         <v>-0.6162838888351784</v>
       </c>
       <c r="F210" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G210" t="n">
         <v>35000</v>
@@ -5294,7 +5294,7 @@
         <v>-0.6326976055089865</v>
       </c>
       <c r="F211" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G211" t="n">
         <v>26000</v>
@@ -5317,7 +5317,7 @@
         <v>-0.5675722135451673</v>
       </c>
       <c r="F212" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G212" t="n">
         <v>60000</v>
@@ -5340,7 +5340,7 @@
         <v>-0.1175186918439774</v>
       </c>
       <c r="F213" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G213" t="n">
         <v>30000</v>
@@ -5363,7 +5363,7 @@
         <v>-0.1175186918439774</v>
       </c>
       <c r="F214" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G214" t="n">
         <v>3000</v>
@@ -5386,7 +5386,7 @@
         <v>-0.5516879716027723</v>
       </c>
       <c r="F215" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G215" t="n">
         <v>25000</v>
@@ -5409,7 +5409,7 @@
         <v>-0.04445117890896069</v>
       </c>
       <c r="F216" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G216" t="n">
         <v>200000</v>
@@ -5432,7 +5432,7 @@
         <v>-0.0529227746115713</v>
       </c>
       <c r="F217" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G217" t="n">
         <v>31500</v>
@@ -5455,7 +5455,7 @@
         <v>-0.4394393285431815</v>
       </c>
       <c r="F218" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G218" t="n">
         <v>15000</v>
@@ -5478,7 +5478,7 @@
         <v>-0.5516879716027723</v>
       </c>
       <c r="F219" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G219" t="n">
         <v>35000</v>
@@ -5501,7 +5501,7 @@
         <v>-0.1339324085177854</v>
       </c>
       <c r="F220" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G220" t="n">
         <v>22000</v>
@@ -5524,7 +5524,7 @@
         <v>2.251880731229934</v>
       </c>
       <c r="F221" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G221" t="n">
         <v>22000</v>
@@ -5547,7 +5547,7 @@
         <v>2.267764973172329</v>
       </c>
       <c r="F222" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G222" t="n">
         <v>43217.5</v>
@@ -5570,7 +5570,7 @@
         <v>1.623394225042508</v>
       </c>
       <c r="F223" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G223" t="n">
         <v>31500</v>
@@ -5593,7 +5593,7 @@
         <v>1.043089919413679</v>
       </c>
       <c r="F224" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G224" t="n">
         <v>40000</v>
@@ -5616,7 +5616,7 @@
         <v>-0.3107769688097825</v>
       </c>
       <c r="F225" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G225" t="n">
         <v>40000</v>
@@ -5639,7 +5639,7 @@
         <v>-0.04445117890896069</v>
       </c>
       <c r="F226" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G226" t="n">
         <v>200000</v>
@@ -5662,7 +5662,7 @@
         <v>-0.04498065364037385</v>
       </c>
       <c r="F227" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G227" t="n">
         <v>40000</v>
@@ -5685,7 +5685,7 @@
         <v>0.334123254051452</v>
       </c>
       <c r="F228" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G228" t="n">
         <v>31500</v>
@@ -5708,7 +5708,7 @@
         <v>-0.04498065364037385</v>
       </c>
       <c r="F229" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G229" t="n">
         <v>40000</v>
@@ -5731,7 +5731,7 @@
         <v>-0.3420159779631591</v>
       </c>
       <c r="F230" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G230" t="n">
         <v>100000</v>
@@ -5754,7 +5754,7 @@
         <v>-0.5998701721613703</v>
       </c>
       <c r="F231" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G231" t="n">
         <v>25000</v>
@@ -5777,7 +5777,7 @@
         <v>-0.3271906854835905</v>
       </c>
       <c r="F232" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G232" t="n">
         <v>200000</v>
@@ -5800,7 +5800,7 @@
         <v>-0.4066118951955652</v>
       </c>
       <c r="F233" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G233" t="n">
         <v>55000</v>
@@ -5823,7 +5823,7 @@
         <v>-0.4717372871593844</v>
       </c>
       <c r="F234" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G234" t="n">
         <v>27000</v>
@@ -5846,7 +5846,7 @@
         <v>-0.3743139365793622</v>
       </c>
       <c r="F235" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G235" t="n">
         <v>38000</v>
@@ -5869,7 +5869,7 @@
         <v>-0.1175186918439774</v>
       </c>
       <c r="F236" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G236" t="n">
         <v>31250</v>
@@ -5892,7 +5892,7 @@
         <v>-0.3584296946369672</v>
       </c>
       <c r="F237" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G237" t="n">
         <v>20000</v>
@@ -5915,7 +5915,7 @@
         <v>-0.3753728860421885</v>
       </c>
       <c r="F238" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G238" t="n">
         <v>35000</v>
@@ -5938,7 +5938,7 @@
         <v>-0.3753728860421885</v>
       </c>
       <c r="F239" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G239" t="n">
         <v>25000</v>
@@ -5961,7 +5961,7 @@
         <v>-0.3753728860421885</v>
       </c>
       <c r="F240" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G240" t="n">
         <v>25000</v>
@@ -5984,7 +5984,7 @@
         <v>-0.3753728860421885</v>
       </c>
       <c r="F241" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G241" t="n">
         <v>25000</v>
@@ -6007,7 +6007,7 @@
         <v>-0.3743139365793622</v>
       </c>
       <c r="F242" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G242" t="n">
         <v>30000</v>
@@ -6030,7 +6030,7 @@
         <v>-0.3743139365793622</v>
       </c>
       <c r="F243" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G243" t="n">
         <v>20000</v>
@@ -6053,7 +6053,7 @@
         <v>-0.3743139365793622</v>
       </c>
       <c r="F244" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G244" t="n">
         <v>30000</v>
@@ -6076,7 +6076,7 @@
         <v>-0.3743139365793622</v>
       </c>
       <c r="F245" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G245" t="n">
         <v>15000</v>
@@ -6099,7 +6099,7 @@
         <v>-0.4394393285431815</v>
       </c>
       <c r="F246" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G246" t="n">
         <v>35000</v>
@@ -6122,7 +6122,7 @@
         <v>-0.5204489624493956</v>
       </c>
       <c r="F247" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G247" t="n">
         <v>35000</v>
@@ -6145,7 +6145,7 @@
         <v>-0.5204489624493956</v>
       </c>
       <c r="F248" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G248" t="n">
         <v>25000</v>
@@ -6168,7 +6168,7 @@
         <v>-0.5204489624493956</v>
       </c>
       <c r="F249" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G249" t="n">
         <v>25000</v>
@@ -6191,7 +6191,7 @@
         <v>-0.5516879716027723</v>
       </c>
       <c r="F250" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G250" t="n">
         <v>30000</v>
@@ -6214,7 +6214,7 @@
         <v>-0.5516879716027723</v>
       </c>
       <c r="F251" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G251" t="n">
         <v>35000</v>
@@ -6237,7 +6237,7 @@
         <v>-0.5998701721613703</v>
       </c>
       <c r="F252" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G252" t="n">
         <v>25000</v>
@@ -6260,7 +6260,7 @@
         <v>-0.5998701721613703</v>
       </c>
       <c r="F253" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G253" t="n">
         <v>30000</v>
@@ -6283,7 +6283,7 @@
         <v>-0.5998701721613703</v>
       </c>
       <c r="F254" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G254" t="n">
         <v>25000</v>
@@ -6306,7 +6306,7 @@
         <v>-0.6162838888351784</v>
       </c>
       <c r="F255" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G255" t="n">
         <v>25000</v>
@@ -6329,7 +6329,7 @@
         <v>-0.6162838888351784</v>
       </c>
       <c r="F256" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G256" t="n">
         <v>25000</v>
@@ -6352,7 +6352,7 @@
         <v>-0.6162838888351784</v>
       </c>
       <c r="F257" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G257" t="n">
         <v>25000</v>
@@ -6375,7 +6375,7 @@
         <v>-0.576043809247778</v>
       </c>
       <c r="F258" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G258" t="n">
         <v>25000</v>
@@ -6398,7 +6398,7 @@
         <v>-0.6485818474513815</v>
       </c>
       <c r="F259" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G259" t="n">
         <v>26000</v>
@@ -6421,7 +6421,7 @@
         <v>-0.6485818474513815</v>
       </c>
       <c r="F260" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G260" t="n">
         <v>26000</v>
@@ -6444,7 +6444,7 @@
         <v>-0.6649955641251896</v>
       </c>
       <c r="F261" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G261" t="n">
         <v>35000</v>
@@ -6467,7 +6467,7 @@
         <v>-0.6649955641251896</v>
       </c>
       <c r="F262" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G262" t="n">
         <v>35000</v>
@@ -6490,7 +6490,7 @@
         <v>-0.6649955641251896</v>
       </c>
       <c r="F263" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G263" t="n">
         <v>30000</v>
@@ -6513,7 +6513,7 @@
         <v>-0.7777736819161936</v>
       </c>
       <c r="F264" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G264" t="n">
         <v>26000</v>
@@ -6534,7 +6534,7 @@
       </c>
       <c r="E265" t="inlineStr"/>
       <c r="F265" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G265" t="n">
         <v>26000</v>
@@ -6557,7 +6557,7 @@
         <v>-0.5516879716027723</v>
       </c>
       <c r="F266" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G266" t="n">
         <v>25000</v>
@@ -6580,7 +6580,7 @@
         <v>-0.5516879716027723</v>
       </c>
       <c r="F267" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G267" t="n">
         <v>25000</v>
@@ -6603,7 +6603,7 @@
         <v>-0.6326976055089865</v>
       </c>
       <c r="F268" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G268" t="n">
         <v>25000</v>
@@ -6626,7 +6626,7 @@
         <v>-0.4733257113536239</v>
       </c>
       <c r="F269" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G269" t="n">
         <v>20000</v>
@@ -6649,7 +6649,7 @@
         <v>-0.4717372871593844</v>
       </c>
       <c r="F270" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G270" t="n">
         <v>25000</v>
@@ -6672,7 +6672,7 @@
         <v>-0.4876215291017794</v>
       </c>
       <c r="F271" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G271" t="n">
         <v>26000</v>
@@ -6695,7 +6695,7 @@
         <v>-0.4876215291017794</v>
       </c>
       <c r="F272" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G272" t="n">
         <v>25000</v>
@@ -6718,7 +6718,7 @@
         <v>-0.7137072394152006</v>
       </c>
       <c r="F273" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G273" t="n">
         <v>26000</v>
@@ -6741,7 +6741,7 @@
         <v>-0.7290620066261825</v>
       </c>
       <c r="F274" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G274" t="n">
         <v>26000</v>
@@ -6764,7 +6764,7 @@
         <v>-0.7290620066261825</v>
       </c>
       <c r="F275" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G275" t="n">
         <v>26000</v>
@@ -6787,7 +6787,7 @@
         <v>-0.7454757232999905</v>
       </c>
       <c r="F276" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G276" t="n">
         <v>26000</v>
@@ -6810,7 +6810,7 @@
         <v>1.494202390577696</v>
       </c>
       <c r="F277" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G277" t="n">
         <v>26250</v>
@@ -6833,7 +6833,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F278" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G278" t="n">
         <v>26250</v>
@@ -6856,7 +6856,7 @@
         <v>-0.1339324085177854</v>
       </c>
       <c r="F279" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G279" t="n">
         <v>25000</v>
@@ -6879,7 +6879,7 @@
         <v>-0.1974693762873652</v>
       </c>
       <c r="F280" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G280" t="n">
         <v>25000</v>
@@ -6902,7 +6902,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F281" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G281" t="n">
         <v>25000</v>
@@ -6925,7 +6925,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F282" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G282" t="n">
         <v>25000</v>
@@ -6948,7 +6948,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F283" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G283" t="n">
         <v>31500</v>
@@ -6971,7 +6971,7 @@
         <v>-0.1175186918439774</v>
       </c>
       <c r="F284" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G284" t="n">
         <v>25000</v>
@@ -6994,7 +6994,7 @@
         <v>-0.2297673349035683</v>
       </c>
       <c r="F285" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G285" t="n">
         <v>22000</v>
@@ -7017,7 +7017,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F286" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G286" t="n">
         <v>31500</v>
@@ -7040,7 +7040,7 @@
         <v>2.284178689846137</v>
       </c>
       <c r="F287" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G287" t="n">
         <v>31500</v>
@@ -7063,7 +7063,7 @@
         <v>-0.1011049751701693</v>
       </c>
       <c r="F288" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G288" t="n">
         <v>20000</v>
@@ -7086,7 +7086,7 @@
         <v>-0.1011049751701693</v>
       </c>
       <c r="F289" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G289" t="n">
         <v>21000</v>
@@ -7109,7 +7109,7 @@
         <v>-0.1974693762873652</v>
       </c>
       <c r="F290" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G290" t="n">
         <v>18000</v>
@@ -7132,7 +7132,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F291" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G291" t="n">
         <v>35000</v>
@@ -7155,7 +7155,7 @@
         <v>-0.2297673349035683</v>
       </c>
       <c r="F292" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G292" t="n">
         <v>22000</v>
@@ -7178,7 +7178,7 @@
         <v>-0.04498065364037385</v>
       </c>
       <c r="F293" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G293" t="n">
         <v>31500</v>
@@ -7201,7 +7201,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F294" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G294" t="n">
         <v>31500</v>
@@ -7224,7 +7224,7 @@
         <v>-0.2297673349035683</v>
       </c>
       <c r="F295" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G295" t="n">
         <v>25000</v>
@@ -7247,7 +7247,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F296" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G296" t="n">
         <v>31500</v>
@@ -7270,7 +7270,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F297" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G297" t="n">
         <v>35000</v>
@@ -7293,7 +7293,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F298" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G298" t="n">
         <v>31500</v>
@@ -7316,7 +7316,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F299" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G299" t="n">
         <v>31500</v>
@@ -7339,7 +7339,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F300" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G300" t="n">
         <v>31500</v>
@@ -7362,7 +7362,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F301" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G301" t="n">
         <v>25000</v>
@@ -7385,7 +7385,7 @@
         <v>-0.3420159779631591</v>
       </c>
       <c r="F302" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G302" t="n">
         <v>25000</v>
@@ -7408,7 +7408,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F303" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G303" t="n">
         <v>31500</v>
@@ -7431,7 +7431,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F304" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G304" t="n">
         <v>22000</v>
@@ -7454,7 +7454,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F305" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G305" t="n">
         <v>25000</v>
@@ -7477,7 +7477,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F306" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G306" t="n">
         <v>20000</v>
@@ -7500,7 +7500,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F307" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G307" t="n">
         <v>22000</v>
@@ -7523,7 +7523,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F308" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G308" t="n">
         <v>31500</v>
@@ -7546,7 +7546,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F309" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G309" t="n">
         <v>25000</v>
@@ -7569,7 +7569,7 @@
         <v>-0.1974693762873652</v>
       </c>
       <c r="F310" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G310" t="n">
         <v>31500</v>
@@ -7592,7 +7592,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F311" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G311" t="n">
         <v>31500</v>
@@ -7615,7 +7615,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F312" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G312" t="n">
         <v>22000</v>
@@ -7638,7 +7638,7 @@
         <v>-0.2133536182297602</v>
       </c>
       <c r="F313" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G313" t="n">
         <v>22000</v>
@@ -7661,7 +7661,7 @@
         <v>-0.4066118951955652</v>
       </c>
       <c r="F314" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G314" t="n">
         <v>19000</v>
@@ -7684,7 +7684,7 @@
         <v>-0.4066118951955652</v>
       </c>
       <c r="F315" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G315" t="n">
         <v>19000</v>
@@ -7707,7 +7707,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F316" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G316" t="n">
         <v>30000</v>
@@ -7730,7 +7730,7 @@
         <v>-0.3933750269102362</v>
       </c>
       <c r="F317" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G317" t="n">
         <v>31500</v>
@@ -7753,7 +7753,7 @@
         <v>-0.2297673349035683</v>
       </c>
       <c r="F318" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G318" t="n">
         <v>31500</v>
@@ -7776,7 +7776,7 @@
         <v>-0.4066118951955652</v>
       </c>
       <c r="F319" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G319" t="n">
         <v>20000</v>
@@ -7799,7 +7799,7 @@
         <v>-0.2133536182297602</v>
       </c>
       <c r="F320" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G320" t="n">
         <v>16000</v>
@@ -7822,7 +7822,7 @@
         <v>-0.2133536182297602</v>
       </c>
       <c r="F321" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G321" t="n">
         <v>22000</v>
@@ -7845,7 +7845,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F322" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G322" t="n">
         <v>31500</v>
@@ -7868,7 +7868,7 @@
         <v>2.235467014556126</v>
       </c>
       <c r="F323" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G323" t="n">
         <v>10000</v>
@@ -7891,7 +7891,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F324" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G324" t="n">
         <v>35000</v>
@@ -7914,7 +7914,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F325" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G325" t="n">
         <v>31000</v>
@@ -7937,7 +7937,7 @@
         <v>-0.4066118951955652</v>
       </c>
       <c r="F326" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G326" t="n">
         <v>25000</v>
@@ -7960,7 +7960,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F327" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G327" t="n">
         <v>31500</v>
@@ -7983,7 +7983,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F328" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G328" t="n">
         <v>25000</v>
@@ -8006,7 +8006,7 @@
         <v>2.10733412955414</v>
       </c>
       <c r="F329" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G329" t="n">
         <v>16684.91</v>
@@ -8029,7 +8029,7 @@
         <v>-0.4066118951955652</v>
       </c>
       <c r="F330" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G330" t="n">
         <v>32000</v>
@@ -8052,7 +8052,7 @@
         <v>-0.4066118951955652</v>
       </c>
       <c r="F331" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G331" t="n">
         <v>20000</v>
@@ -8075,7 +8075,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F332" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G332" t="n">
         <v>31500</v>
@@ -8098,7 +8098,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F333" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G333" t="n">
         <v>31500</v>
@@ -8121,7 +8121,7 @@
         <v>-0.1175186918439774</v>
       </c>
       <c r="F334" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G334" t="n">
         <v>31500</v>
@@ -8144,7 +8144,7 @@
         <v>-0.1974693762873652</v>
       </c>
       <c r="F335" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G335" t="n">
         <v>25000</v>
@@ -8167,7 +8167,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F336" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G336" t="n">
         <v>31500</v>
@@ -8190,7 +8190,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F337" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G337" t="n">
         <v>25000</v>
@@ -8213,7 +8213,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F338" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G338" t="n">
         <v>25000</v>
@@ -8236,7 +8236,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F339" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G339" t="n">
         <v>31500</v>
@@ -8259,7 +8259,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F340" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G340" t="n">
         <v>22000</v>
@@ -8282,7 +8282,7 @@
         <v>-0.1974693762873652</v>
       </c>
       <c r="F341" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G341" t="n">
         <v>35000</v>
@@ -8305,7 +8305,7 @@
         <v>-0.1974693762873652</v>
       </c>
       <c r="F342" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G342" t="n">
         <v>20000</v>
@@ -8328,7 +8328,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F343" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G343" t="n">
         <v>31500</v>
@@ -8351,7 +8351,7 @@
         <v>-0.1175186918439774</v>
       </c>
       <c r="F344" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G344" t="n">
         <v>20000</v>
@@ -8374,7 +8374,7 @@
         <v>-0.08522073322777438</v>
       </c>
       <c r="F345" t="n">
-        <v>0</v>
+        <v>35003.84593023256</v>
       </c>
       <c r="G345" t="n">
         <v>22000</v>

</xml_diff>